<commit_message>
added testing only equalities and fixed bug in calculation of G
</commit_message>
<xml_diff>
--- a/results/results-sizes.xlsx
+++ b/results/results-sizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils\Documents\Studium\TUM\09_Masterarbeit\master-thesis-tests\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EB508D-9FB8-47E1-8E80-8DBE7D9AE604}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA236793-381F-4A18-AE7C-8A4AA81C05BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="-1968" windowWidth="19392" windowHeight="10392" xr2:uid="{10A37585-0CE9-42C1-8EEA-BBFDD8762655}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10A37585-0CE9-42C1-8EEA-BBFDD8762655}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>m = 20</t>
   </si>
@@ -62,6 +62,9 @@
   <si>
     <t>Test 3</t>
   </si>
+  <si>
+    <t>ok</t>
+  </si>
 </sst>
 </file>
 
@@ -69,7 +72,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -295,6 +298,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -307,43 +346,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -663,7 +666,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,28 +682,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="22" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="22" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
       <c r="O1" s="15"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -749,7 +752,7 @@
       <c r="O2" s="15"/>
     </row>
     <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
+      <c r="A3" s="30">
         <v>100</v>
       </c>
       <c r="B3" s="2">
@@ -758,7 +761,7 @@
       <c r="C3" s="8">
         <v>6.2E-2</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="24">
         <v>0.3</v>
       </c>
       <c r="E3" s="8"/>
@@ -775,14 +778,20 @@
       <c r="J3" s="10">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="14"/>
+      <c r="K3" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
+      <c r="N3" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="O3" s="15"/>
     </row>
     <row r="4" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="2">
         <v>0.05</v>
       </c>
@@ -793,7 +802,7 @@
         <v>0.69799999999999995</v>
       </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="27">
+      <c r="F4" s="20">
         <v>0.05</v>
       </c>
       <c r="G4" s="9">
@@ -806,14 +815,16 @@
       <c r="J4" s="10">
         <v>0.13400000000000001</v>
       </c>
-      <c r="K4" s="9"/>
+      <c r="K4" s="9">
+        <v>0.216</v>
+      </c>
       <c r="L4" s="14"/>
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
       <c r="O4" s="15"/>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="3">
         <v>0.1</v>
       </c>
@@ -834,23 +845,25 @@
         <v>0.95799999999999996</v>
       </c>
       <c r="I5" s="11"/>
-      <c r="J5" s="34">
+      <c r="J5" s="27">
         <v>0.21</v>
       </c>
-      <c r="K5" s="12"/>
+      <c r="K5" s="12">
+        <v>0.42</v>
+      </c>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
       <c r="O5" s="15"/>
     </row>
     <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+      <c r="A6" s="30">
         <v>250</v>
       </c>
       <c r="B6" s="2">
         <v>0.01</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="20">
         <v>0.01</v>
       </c>
       <c r="D6" s="8">
@@ -860,7 +873,7 @@
       <c r="F6" s="8">
         <v>1.2E-2</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="19">
         <v>0.01</v>
       </c>
       <c r="H6" s="14">
@@ -870,14 +883,16 @@
       <c r="J6" s="10">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="K6" s="9"/>
+      <c r="K6" s="9">
+        <v>2E-3</v>
+      </c>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
       <c r="O6" s="15"/>
     </row>
     <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="2">
         <v>0.05</v>
       </c>
@@ -898,17 +913,19 @@
         <v>0.21199999999999999</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="32">
+      <c r="J7" s="25">
         <v>0.27</v>
       </c>
-      <c r="K7" s="9"/>
+      <c r="K7" s="9">
+        <v>3.7999999999999999E-2</v>
+      </c>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
       <c r="O7" s="15"/>
     </row>
     <row r="8" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="3">
         <v>0.1</v>
       </c>
@@ -922,7 +939,7 @@
       <c r="F8" s="11">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="18">
         <v>0.11</v>
       </c>
       <c r="H8" s="11">
@@ -932,14 +949,16 @@
       <c r="J8" s="13">
         <v>0.39800000000000002</v>
       </c>
-      <c r="K8" s="12"/>
+      <c r="K8" s="12">
+        <v>8.4000000000000005E-2</v>
+      </c>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="15"/>
     </row>
     <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="30">
         <v>500</v>
       </c>
       <c r="B9" s="2">
@@ -955,7 +974,7 @@
       <c r="F9" s="8">
         <v>1.2E-2</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="19">
         <v>0.01</v>
       </c>
       <c r="H9" s="14">
@@ -965,18 +984,20 @@
       <c r="J9" s="10">
         <v>0.36799999999999999</v>
       </c>
-      <c r="K9" s="9"/>
+      <c r="K9" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
       <c r="O9" s="15"/>
     </row>
     <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="2">
         <v>0.05</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="20">
         <v>0.02</v>
       </c>
       <c r="D10" s="8">
@@ -986,7 +1007,7 @@
       <c r="F10" s="8">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="19">
         <v>0.03</v>
       </c>
       <c r="H10" s="14">
@@ -996,45 +1017,49 @@
       <c r="J10" s="10">
         <v>0.626</v>
       </c>
-      <c r="K10" s="9"/>
+      <c r="K10" s="9">
+        <v>3.2000000000000001E-2</v>
+      </c>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
       <c r="O10" s="15"/>
     </row>
     <row r="11" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="3">
         <v>0.1</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="21">
         <v>0.06</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="21">
         <v>0.09</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11">
         <v>0.10199999999999999</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="18">
         <v>0.08</v>
       </c>
       <c r="H11" s="11">
         <v>0.124</v>
       </c>
       <c r="I11" s="11"/>
-      <c r="J11" s="34">
+      <c r="J11" s="27">
         <v>0.74</v>
       </c>
-      <c r="K11" s="12"/>
+      <c r="K11" s="12">
+        <v>5.8000000000000003E-2</v>
+      </c>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="15"/>
     </row>
     <row r="12" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="A12" s="30">
         <v>1000</v>
       </c>
       <c r="B12" s="2">
@@ -1056,20 +1081,22 @@
       <c r="H12" s="14">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="23">
         <v>0</v>
       </c>
       <c r="J12" s="10">
         <v>0.85599999999999998</v>
       </c>
-      <c r="K12" s="9"/>
+      <c r="K12" s="9">
+        <v>2E-3</v>
+      </c>
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
       <c r="N12" s="14"/>
       <c r="O12" s="15"/>
     </row>
     <row r="13" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="2">
         <v>0.05</v>
       </c>
@@ -1083,26 +1110,28 @@
       <c r="F13" s="8">
         <v>6.2E-2</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="19">
         <v>0.03</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="22">
         <v>0.04</v>
       </c>
-      <c r="I13" s="29">
+      <c r="I13" s="22">
         <v>0.03</v>
       </c>
       <c r="J13" s="10">
         <v>0.94399999999999995</v>
       </c>
-      <c r="K13" s="9"/>
+      <c r="K13" s="9">
+        <v>2.5999999999999999E-2</v>
+      </c>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
       <c r="O13" s="15"/>
     </row>
     <row r="14" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="3">
         <v>0.1</v>
       </c>
@@ -1128,14 +1157,16 @@
       <c r="J14" s="13">
         <v>0.96199999999999997</v>
       </c>
-      <c r="K14" s="12"/>
+      <c r="K14" s="12">
+        <v>6.6000000000000003E-2</v>
+      </c>
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
       <c r="O14" s="15"/>
     </row>
     <row r="15" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
+      <c r="A15" s="30">
         <v>2000</v>
       </c>
       <c r="B15" s="2">
@@ -1158,24 +1189,26 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="I15" s="14"/>
-      <c r="J15" s="33">
+      <c r="J15" s="26">
         <v>1</v>
       </c>
-      <c r="K15" s="9"/>
+      <c r="K15" s="9">
+        <v>2E-3</v>
+      </c>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
       <c r="O15" s="15"/>
     </row>
     <row r="16" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="2">
         <v>0.05</v>
       </c>
       <c r="C16" s="8">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="20">
         <v>0.03</v>
       </c>
       <c r="E16" s="8"/>
@@ -1189,24 +1222,26 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="I16" s="14"/>
-      <c r="J16" s="33">
+      <c r="J16" s="26">
         <v>1</v>
       </c>
-      <c r="K16" s="9"/>
+      <c r="K16" s="9">
+        <v>1.6E-2</v>
+      </c>
       <c r="L16" s="14"/>
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
       <c r="O16" s="15"/>
     </row>
     <row r="17" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="2">
         <v>0.1</v>
       </c>
-      <c r="C17" s="29">
+      <c r="C17" s="22">
         <v>0.08</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="22">
         <v>0.06</v>
       </c>
       <c r="E17" s="14"/>
@@ -1220,10 +1255,12 @@
         <v>0.104</v>
       </c>
       <c r="I17" s="14"/>
-      <c r="J17" s="33">
+      <c r="J17" s="26">
         <v>1</v>
       </c>
-      <c r="K17" s="9"/>
+      <c r="K17" s="9">
+        <v>4.2000000000000003E-2</v>
+      </c>
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
@@ -1248,7 +1285,6 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
@@ -1257,8 +1293,9 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A3:A5"/>
+    <mergeCell ref="G1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
experiments on high-dimensional setup
</commit_message>
<xml_diff>
--- a/results/results-sizes.xlsx
+++ b/results/results-sizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils\Documents\Studium\TUM\09_Masterarbeit\master-thesis-tests\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA9CFA3-02CF-4A86-93CE-9493893E28FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC05CE0-AB0A-43E3-9D38-0E1FCD8DB887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10A37585-0CE9-42C1-8EEA-BBFDD8762655}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="28770" windowHeight="15600" xr2:uid="{10A37585-0CE9-42C1-8EEA-BBFDD8762655}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -331,6 +331,15 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -351,15 +360,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,28 +694,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="28" t="s">
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="28" t="s">
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
       <c r="O1" s="15"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
       <c r="O2" s="15"/>
     </row>
     <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30">
+      <c r="A3" s="33">
         <v>100</v>
       </c>
       <c r="B3" s="2">
@@ -797,13 +797,13 @@
         <v>0.44600000000000001</v>
       </c>
       <c r="M3" s="14"/>
-      <c r="N3" s="35">
+      <c r="N3" s="28">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="O3" s="15"/>
     </row>
     <row r="4" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="2">
         <v>0.05</v>
       </c>
@@ -840,7 +840,7 @@
       <c r="O4" s="15"/>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="3">
         <v>0.1</v>
       </c>
@@ -871,13 +871,13 @@
         <v>0.92</v>
       </c>
       <c r="M5" s="11"/>
-      <c r="N5" s="37">
+      <c r="N5" s="30">
         <v>0.37</v>
       </c>
       <c r="O5" s="15"/>
     </row>
     <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30">
+      <c r="A6" s="33">
         <v>250</v>
       </c>
       <c r="B6" s="2">
@@ -910,12 +910,12 @@
         <v>0.20799999999999999</v>
       </c>
       <c r="M6" s="14"/>
-      <c r="N6" s="36">
+      <c r="N6" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="2">
         <v>0.05</v>
       </c>
@@ -952,7 +952,7 @@
       <c r="O7" s="15"/>
     </row>
     <row r="8" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="3">
         <v>0.1</v>
       </c>
@@ -983,13 +983,13 @@
         <v>0.38200000000000001</v>
       </c>
       <c r="M8" s="11"/>
-      <c r="N8" s="37">
+      <c r="N8" s="30">
         <v>0.16</v>
       </c>
       <c r="O8" s="15"/>
     </row>
     <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30">
+      <c r="A9" s="33">
         <v>500</v>
       </c>
       <c r="B9" s="2">
@@ -1028,7 +1028,7 @@
       <c r="O9" s="15"/>
     </row>
     <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="2">
         <v>0.05</v>
       </c>
@@ -1065,7 +1065,7 @@
       <c r="O10" s="15"/>
     </row>
     <row r="11" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="3">
         <v>0.1</v>
       </c>
@@ -1096,13 +1096,13 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="M11" s="11"/>
-      <c r="N11" s="37">
+      <c r="N11" s="30">
         <v>0.08</v>
       </c>
       <c r="O11" s="15"/>
     </row>
     <row r="12" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
+      <c r="A12" s="33">
         <v>1000</v>
       </c>
       <c r="B12" s="2">
@@ -1143,7 +1143,7 @@
       <c r="O12" s="15"/>
     </row>
     <row r="13" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="2">
         <v>0.05</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="O13" s="15"/>
     </row>
     <row r="14" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="3">
         <v>0.1</v>
       </c>
@@ -1215,13 +1215,13 @@
         <v>0.106</v>
       </c>
       <c r="M14" s="11"/>
-      <c r="N14" s="37">
+      <c r="N14" s="30">
         <v>0.08</v>
       </c>
       <c r="O14" s="15"/>
     </row>
     <row r="15" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30">
+      <c r="A15" s="33">
         <v>2000</v>
       </c>
       <c r="B15" s="2">
@@ -1257,7 +1257,7 @@
       <c r="O15" s="15"/>
     </row>
     <row r="16" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="2">
         <v>0.05</v>
       </c>
@@ -1291,7 +1291,7 @@
       <c r="O16" s="15"/>
     </row>
     <row r="17" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="2">
         <v>0.1</v>
       </c>

</xml_diff>

<commit_message>
finished table result sizes
</commit_message>
<xml_diff>
--- a/results/results-sizes.xlsx
+++ b/results/results-sizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils\Documents\Studium\TUM\09_Masterarbeit\master-thesis-tests\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC05CE0-AB0A-43E3-9D38-0E1FCD8DB887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA6BB95-AE2F-425E-A268-3D684212C026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="28770" windowHeight="15600" xr2:uid="{10A37585-0CE9-42C1-8EEA-BBFDD8762655}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10A37585-0CE9-42C1-8EEA-BBFDD8762655}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>α</t>
   </si>
   <si>
-    <t>star tree setup 1</t>
-  </si>
-  <si>
     <t>LR</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   <si>
     <t>Test 3</t>
   </si>
+  <si>
+    <t>star tree - setup 1</t>
+  </si>
 </sst>
 </file>
 
@@ -71,7 +71,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,12 +100,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -250,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -331,15 +325,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -359,6 +344,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -677,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DE9B96-2516-48F5-9B22-0E368715A17B}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,28 +685,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="31" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
       <c r="O1" s="15"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -726,45 +717,45 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="J2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="N2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O2" s="15"/>
     </row>
     <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33">
+      <c r="A3" s="30">
         <v>100</v>
       </c>
       <c r="B3" s="2">
@@ -776,7 +767,9 @@
       <c r="D3" s="24">
         <v>0.3</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="36">
+        <v>0</v>
+      </c>
       <c r="F3" s="8">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -786,7 +779,9 @@
       <c r="H3" s="14">
         <v>0.41799999999999998</v>
       </c>
-      <c r="I3" s="14"/>
+      <c r="I3" s="23">
+        <v>0</v>
+      </c>
       <c r="J3" s="10">
         <v>3.4000000000000002E-2</v>
       </c>
@@ -796,14 +791,16 @@
       <c r="L3" s="14">
         <v>0.44600000000000001</v>
       </c>
-      <c r="M3" s="14"/>
-      <c r="N3" s="28">
+      <c r="M3" s="23">
+        <v>0</v>
+      </c>
+      <c r="N3" s="14">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="O3" s="15"/>
     </row>
     <row r="4" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="2">
         <v>0.05</v>
       </c>
@@ -813,7 +810,9 @@
       <c r="D4" s="8">
         <v>0.69799999999999995</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="8">
+        <v>2E-3</v>
+      </c>
       <c r="F4" s="20">
         <v>0.05</v>
       </c>
@@ -823,7 +822,9 @@
       <c r="H4" s="14">
         <v>0.85599999999999998</v>
       </c>
-      <c r="I4" s="14"/>
+      <c r="I4" s="23">
+        <v>0</v>
+      </c>
       <c r="J4" s="10">
         <v>0.13400000000000001</v>
       </c>
@@ -833,14 +834,16 @@
       <c r="L4" s="22">
         <v>0.78</v>
       </c>
-      <c r="M4" s="14"/>
-      <c r="N4" s="1">
+      <c r="M4" s="23">
+        <v>0</v>
+      </c>
+      <c r="N4" s="14">
         <v>0.24399999999999999</v>
       </c>
       <c r="O4" s="15"/>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="3">
         <v>0.1</v>
       </c>
@@ -850,7 +853,9 @@
       <c r="D5" s="11">
         <v>0.88400000000000001</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="11">
+        <v>8.0000000000000002E-3</v>
+      </c>
       <c r="F5" s="11">
         <v>9.1999999999999998E-2</v>
       </c>
@@ -860,7 +865,9 @@
       <c r="H5" s="11">
         <v>0.95799999999999996</v>
       </c>
-      <c r="I5" s="11"/>
+      <c r="I5" s="35">
+        <v>0</v>
+      </c>
       <c r="J5" s="27">
         <v>0.21</v>
       </c>
@@ -870,14 +877,16 @@
       <c r="L5" s="21">
         <v>0.92</v>
       </c>
-      <c r="M5" s="11"/>
-      <c r="N5" s="30">
+      <c r="M5" s="35">
+        <v>0</v>
+      </c>
+      <c r="N5" s="21">
         <v>0.37</v>
       </c>
       <c r="O5" s="15"/>
     </row>
     <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33">
+      <c r="A6" s="30">
         <v>250</v>
       </c>
       <c r="B6" s="2">
@@ -889,7 +898,9 @@
       <c r="D6" s="8">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="36">
+        <v>0</v>
+      </c>
       <c r="F6" s="8">
         <v>1.2E-2</v>
       </c>
@@ -899,7 +910,9 @@
       <c r="H6" s="14">
         <v>0.10199999999999999</v>
       </c>
-      <c r="I6" s="14"/>
+      <c r="I6" s="23">
+        <v>0</v>
+      </c>
       <c r="J6" s="10">
         <v>8.7999999999999995E-2</v>
       </c>
@@ -909,13 +922,15 @@
       <c r="L6" s="14">
         <v>0.20799999999999999</v>
       </c>
-      <c r="M6" s="14"/>
-      <c r="N6" s="29">
+      <c r="M6" s="23">
         <v>0</v>
       </c>
+      <c r="N6" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="2">
         <v>0.05</v>
       </c>
@@ -925,7 +940,9 @@
       <c r="D7" s="8">
         <v>0.13600000000000001</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
       <c r="F7" s="8">
         <v>4.2000000000000003E-2</v>
       </c>
@@ -935,7 +952,9 @@
       <c r="H7" s="14">
         <v>0.21199999999999999</v>
       </c>
-      <c r="I7" s="14"/>
+      <c r="I7" s="14">
+        <v>2.5999999999999999E-2</v>
+      </c>
       <c r="J7" s="25">
         <v>0.27</v>
       </c>
@@ -945,14 +964,16 @@
       <c r="L7" s="14">
         <v>0.30199999999999999</v>
       </c>
-      <c r="M7" s="14"/>
-      <c r="N7" s="1">
+      <c r="M7" s="23">
+        <v>0</v>
+      </c>
+      <c r="N7" s="22">
         <v>0.12</v>
       </c>
       <c r="O7" s="15"/>
     </row>
     <row r="8" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="3">
         <v>0.1</v>
       </c>
@@ -962,7 +983,9 @@
       <c r="D8" s="11">
         <v>0.24199999999999999</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="11">
+        <v>2.1999999999999999E-2</v>
+      </c>
       <c r="F8" s="11">
         <v>8.7999999999999995E-2</v>
       </c>
@@ -972,7 +995,9 @@
       <c r="H8" s="11">
         <v>0.32600000000000001</v>
       </c>
-      <c r="I8" s="11"/>
+      <c r="I8" s="11">
+        <v>5.3999999999999999E-2</v>
+      </c>
       <c r="J8" s="13">
         <v>0.39800000000000002</v>
       </c>
@@ -982,14 +1007,16 @@
       <c r="L8" s="11">
         <v>0.38200000000000001</v>
       </c>
-      <c r="M8" s="11"/>
-      <c r="N8" s="30">
+      <c r="M8" s="11">
+        <v>2E-3</v>
+      </c>
+      <c r="N8" s="21">
         <v>0.16</v>
       </c>
       <c r="O8" s="15"/>
     </row>
     <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33">
+      <c r="A9" s="30">
         <v>500</v>
       </c>
       <c r="B9" s="2">
@@ -1001,7 +1028,9 @@
       <c r="D9" s="8">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="36">
+        <v>0</v>
+      </c>
       <c r="F9" s="8">
         <v>1.2E-2</v>
       </c>
@@ -1011,7 +1040,9 @@
       <c r="H9" s="14">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="I9" s="14"/>
+      <c r="I9" s="14">
+        <v>6.0000000000000001E-3</v>
+      </c>
       <c r="J9" s="10">
         <v>0.36799999999999999</v>
       </c>
@@ -1021,14 +1052,16 @@
       <c r="L9" s="14">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="M9" s="14"/>
-      <c r="N9" s="1">
+      <c r="M9" s="14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="N9" s="22">
         <v>0.06</v>
       </c>
       <c r="O9" s="15"/>
     </row>
     <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="2">
         <v>0.05</v>
       </c>
@@ -1038,7 +1071,9 @@
       <c r="D10" s="8">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8">
+        <v>2.1999999999999999E-2</v>
+      </c>
       <c r="F10" s="8">
         <v>4.5999999999999999E-2</v>
       </c>
@@ -1048,7 +1083,9 @@
       <c r="H10" s="14">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="I10" s="14"/>
+      <c r="I10" s="14">
+        <v>4.5999999999999999E-2</v>
+      </c>
       <c r="J10" s="10">
         <v>0.626</v>
       </c>
@@ -1058,14 +1095,16 @@
       <c r="L10" s="14">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="M10" s="14"/>
-      <c r="N10" s="1">
+      <c r="M10" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N10" s="22">
         <v>0.04</v>
       </c>
       <c r="O10" s="15"/>
     </row>
     <row r="11" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="3">
         <v>0.1</v>
       </c>
@@ -1075,7 +1114,9 @@
       <c r="D11" s="21">
         <v>0.09</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="11">
+        <v>4.3999999999999997E-2</v>
+      </c>
       <c r="F11" s="11">
         <v>0.10199999999999999</v>
       </c>
@@ -1085,7 +1126,9 @@
       <c r="H11" s="11">
         <v>0.124</v>
       </c>
-      <c r="I11" s="11"/>
+      <c r="I11" s="11">
+        <v>7.3999999999999996E-2</v>
+      </c>
       <c r="J11" s="27">
         <v>0.74</v>
       </c>
@@ -1095,14 +1138,16 @@
       <c r="L11" s="11">
         <v>0.11600000000000001</v>
       </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="30">
+      <c r="M11" s="11">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N11" s="21">
         <v>0.08</v>
       </c>
       <c r="O11" s="15"/>
     </row>
     <row r="12" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="33">
+      <c r="A12" s="30">
         <v>1000</v>
       </c>
       <c r="B12" s="2">
@@ -1114,7 +1159,9 @@
       <c r="D12" s="8">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8">
+        <v>0.01</v>
+      </c>
       <c r="F12" s="8">
         <v>1.2E-2</v>
       </c>
@@ -1124,8 +1171,8 @@
       <c r="H12" s="14">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="I12" s="23">
-        <v>0</v>
+      <c r="I12" s="14">
+        <v>1.2E-2</v>
       </c>
       <c r="J12" s="10">
         <v>0.85599999999999998</v>
@@ -1136,14 +1183,16 @@
       <c r="L12" s="14">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="M12" s="14"/>
-      <c r="N12" s="7">
+      <c r="M12" s="23">
+        <v>0</v>
+      </c>
+      <c r="N12" s="14">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="O12" s="15"/>
     </row>
     <row r="13" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="2">
         <v>0.05</v>
       </c>
@@ -1153,7 +1202,9 @@
       <c r="D13" s="8">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8">
+        <v>2.4E-2</v>
+      </c>
       <c r="F13" s="8">
         <v>6.2E-2</v>
       </c>
@@ -1163,8 +1214,8 @@
       <c r="H13" s="22">
         <v>0.04</v>
       </c>
-      <c r="I13" s="22">
-        <v>0.03</v>
+      <c r="I13" s="14">
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="J13" s="10">
         <v>0.94399999999999995</v>
@@ -1175,14 +1226,16 @@
       <c r="L13" s="22">
         <v>0.06</v>
       </c>
-      <c r="M13" s="14"/>
-      <c r="N13" s="1">
+      <c r="M13" s="14">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N13" s="14">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="O13" s="15"/>
     </row>
     <row r="14" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="3">
         <v>0.1</v>
       </c>
@@ -1192,7 +1245,9 @@
       <c r="D14" s="11">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="11">
+        <v>6.2E-2</v>
+      </c>
       <c r="F14" s="11">
         <v>0.11</v>
       </c>
@@ -1202,8 +1257,8 @@
       <c r="H14" s="11">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="I14" s="11">
-        <v>7.8E-2</v>
+      <c r="I14" s="21">
+        <v>0.11</v>
       </c>
       <c r="J14" s="13">
         <v>0.96199999999999997</v>
@@ -1214,14 +1269,16 @@
       <c r="L14" s="11">
         <v>0.106</v>
       </c>
-      <c r="M14" s="11"/>
-      <c r="N14" s="30">
+      <c r="M14" s="11">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="N14" s="21">
         <v>0.08</v>
       </c>
       <c r="O14" s="15"/>
     </row>
     <row r="15" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33">
+      <c r="A15" s="30">
         <v>2000</v>
       </c>
       <c r="B15" s="2">
@@ -1257,7 +1314,7 @@
       <c r="O15" s="15"/>
     </row>
     <row r="16" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="2">
         <v>0.05</v>
       </c>
@@ -1291,7 +1348,7 @@
       <c r="O16" s="15"/>
     </row>
     <row r="17" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="2">
         <v>0.1</v>
       </c>
@@ -1354,6 +1411,6 @@
     <mergeCell ref="G1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>